<commit_message>
Added an option similarProductsInFirstCycleEnabled to evaluationWithNominal.py;  which shows similar products (similar to query) in the first cycle, instead of showing top K products according to initial utility model. The hunch is that critique strings will be more overlapping in the first iteration and they are customized to every product/query. Showing the same 5 products 196,1,178..  always is not customized to each query/product
</commit_message>
<xml_diff>
--- a/src/Results.xlsx
+++ b/src/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>limitations:</t>
   </si>
@@ -95,6 +95,9 @@
   <si>
     <t>allAttributesTowardsTarget</t>
   </si>
+  <si>
+    <t>similarProductsIn FirstCycle</t>
+  </si>
 </sst>
 </file>
 
@@ -141,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -173,19 +176,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -233,8 +225,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -261,9 +261,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -287,6 +292,10 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -310,6 +319,10 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -377,7 +390,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>11.8</c:v>
+                  <c:v>12.24</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.82</c:v>
@@ -428,7 +441,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12.14</c:v>
+                  <c:v>12.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.92</c:v>
@@ -482,7 +495,7 @@
                   <c:v>12.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>4.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.42</c:v>
@@ -500,7 +513,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>updateWeightsWrtInitialPreferences</c:v>
+                  <c:v>similarProductsIn FirstCycle</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -530,7 +543,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9.12</c:v>
+                  <c:v>6.56</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -551,7 +564,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>attributesInLineWithTarget</c:v>
+                  <c:v>updateWeightsWrtInitialPreferences</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -581,7 +594,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.37</c:v>
+                  <c:v>9.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -596,7 +615,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>allAttributesTowardsTarget</c:v>
+                  <c:v>attributesInLineWithTarget</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -622,6 +641,51 @@
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>allAttributesTowardsTarget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -641,11 +705,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="519365576"/>
-        <c:axId val="519370488"/>
+        <c:axId val="562139640"/>
+        <c:axId val="562128152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="519365576"/>
+        <c:axId val="562139640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,7 +718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519370488"/>
+        <c:crossAx val="562128152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -662,7 +726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="519370488"/>
+        <c:axId val="562128152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -673,7 +737,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519365576"/>
+        <c:crossAx val="562139640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -721,7 +785,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$12</c:f>
+              <c:f>Sheet1!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -733,7 +797,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$11:$D$11</c:f>
+              <c:f>Sheet1!$B$13:$D$13</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -750,7 +814,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$D$12</c:f>
+              <c:f>Sheet1!$B$14:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -772,7 +836,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$13</c:f>
+              <c:f>Sheet1!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -784,7 +848,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$11:$D$11</c:f>
+              <c:f>Sheet1!$B$13:$D$13</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -801,7 +865,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:f>Sheet1!$B$15:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -823,7 +887,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$14</c:f>
+              <c:f>Sheet1!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -835,7 +899,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$11:$D$11</c:f>
+              <c:f>Sheet1!$B$13:$D$13</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -852,7 +916,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$D$14</c:f>
+              <c:f>Sheet1!$B$16:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -878,11 +942,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="519446104"/>
-        <c:axId val="519449080"/>
+        <c:axId val="579919160"/>
+        <c:axId val="579922136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="519446104"/>
+        <c:axId val="579919160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +955,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519449080"/>
+        <c:crossAx val="579922136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -899,7 +963,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="519449080"/>
+        <c:axId val="579922136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -910,7 +974,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519446104"/>
+        <c:crossAx val="579919160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -958,7 +1022,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$34</c:f>
+              <c:f>Sheet1!$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -970,7 +1034,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$33:$D$33</c:f>
+              <c:f>Sheet1!$B$35:$D$35</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -987,7 +1051,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$34:$D$34</c:f>
+              <c:f>Sheet1!$B$36:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1009,7 +1073,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$35</c:f>
+              <c:f>Sheet1!$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1021,7 +1085,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$33:$D$33</c:f>
+              <c:f>Sheet1!$B$35:$D$35</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1038,7 +1102,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$35:$D$35</c:f>
+              <c:f>Sheet1!$B$37:$D$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1060,7 +1124,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$36</c:f>
+              <c:f>Sheet1!$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1072,7 +1136,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$33:$D$33</c:f>
+              <c:f>Sheet1!$B$35:$D$35</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1089,7 +1153,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$36:$D$36</c:f>
+              <c:f>Sheet1!$B$38:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1106,11 +1170,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="519479624"/>
-        <c:axId val="519482600"/>
+        <c:axId val="579952792"/>
+        <c:axId val="579955768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="519479624"/>
+        <c:axId val="579952792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1119,7 +1183,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519482600"/>
+        <c:crossAx val="579955768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1127,7 +1191,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="519482600"/>
+        <c:axId val="579955768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1138,7 +1202,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519479624"/>
+        <c:crossAx val="579952792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1186,7 +1250,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$41</c:f>
+              <c:f>Sheet1!$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1198,7 +1262,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$40:$D$40</c:f>
+              <c:f>Sheet1!$B$42:$D$42</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1215,7 +1279,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$41:$D$41</c:f>
+              <c:f>Sheet1!$B$43:$D$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1237,7 +1301,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$42</c:f>
+              <c:f>Sheet1!$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1249,7 +1313,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$40:$D$40</c:f>
+              <c:f>Sheet1!$B$42:$D$42</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1266,7 +1330,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$42:$D$42</c:f>
+              <c:f>Sheet1!$B$44:$D$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1288,7 +1352,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$43</c:f>
+              <c:f>Sheet1!$A$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1300,7 +1364,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$40:$D$40</c:f>
+              <c:f>Sheet1!$B$42:$D$42</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1317,7 +1381,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$D$43</c:f>
+              <c:f>Sheet1!$B$45:$D$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1343,11 +1407,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="519513576"/>
-        <c:axId val="519516552"/>
+        <c:axId val="579986696"/>
+        <c:axId val="579989672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="519513576"/>
+        <c:axId val="579986696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1356,7 +1420,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519516552"/>
+        <c:crossAx val="579989672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1364,7 +1428,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="519516552"/>
+        <c:axId val="579989672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1375,7 +1439,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519513576"/>
+        <c:crossAx val="579986696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1423,7 +1487,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$19</c:f>
+              <c:f>Sheet1!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1435,7 +1499,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$18:$D$18</c:f>
+              <c:f>Sheet1!$B$20:$D$20</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1452,7 +1516,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$D$19</c:f>
+              <c:f>Sheet1!$B$21:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1468,7 +1532,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$20</c:f>
+              <c:f>Sheet1!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1480,7 +1544,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$18:$D$18</c:f>
+              <c:f>Sheet1!$B$20:$D$20</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1497,7 +1561,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$20:$D$20</c:f>
+              <c:f>Sheet1!$B$22:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1513,7 +1577,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$21</c:f>
+              <c:f>Sheet1!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1525,7 +1589,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$18:$D$18</c:f>
+              <c:f>Sheet1!$B$20:$D$20</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1542,7 +1606,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$21:$D$21</c:f>
+              <c:f>Sheet1!$B$23:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1559,11 +1623,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="519547656"/>
-        <c:axId val="519550632"/>
+        <c:axId val="580021336"/>
+        <c:axId val="580024312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="519547656"/>
+        <c:axId val="580021336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1572,7 +1636,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519550632"/>
+        <c:crossAx val="580024312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1580,7 +1644,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="519550632"/>
+        <c:axId val="580024312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,7 +1655,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519547656"/>
+        <c:crossAx val="580021336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1649,13 +1713,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>420413</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>122614</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2417378</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>157655</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1679,13 +1743,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>613103</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>116928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2312276</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>131380</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1709,13 +1773,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>604344</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>122621</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2338551</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>183931</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1739,13 +1803,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>437930</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>832069</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2601309</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>149771</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2090,10 +2154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:R48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2161,7 +2225,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="4">
-        <v>11.8</v>
+        <v>12.24</v>
       </c>
       <c r="C3" s="4">
         <v>4.82</v>
@@ -2175,7 +2239,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="4">
-        <v>12.14</v>
+        <v>12.2</v>
       </c>
       <c r="C4" s="4">
         <v>4.92</v>
@@ -2192,18 +2256,18 @@
         <v>12.02</v>
       </c>
       <c r="C5" s="4">
-        <v>0</v>
+        <v>4.84</v>
       </c>
       <c r="D5" s="4">
         <v>2.42</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="30">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
+      <c r="A6" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B6" s="10">
-        <v>9.1199999999999992</v>
+        <v>6.56</v>
       </c>
       <c r="C6" s="10">
         <v>0</v>
@@ -2213,262 +2277,286 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="30">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="10">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="30">
+      <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B8" s="10">
         <v>3.37</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="30">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" ht="30">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B9" s="10">
         <v>2.15</v>
       </c>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="3" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="6" t="s">
+    <row r="14" spans="1:18">
+      <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B14" s="4">
         <v>10.37</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C14" s="4">
         <v>4.5199999999999996</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D14" s="4">
         <v>2.27</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="30">
-      <c r="A13" s="6" t="s">
+    <row r="15" spans="1:18" ht="30">
+      <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B15" s="4">
         <v>10.3</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C15" s="4">
         <v>4.2</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D15" s="4">
         <v>2.02</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="2" customFormat="1" ht="45">
-      <c r="A14" s="6" t="s">
+    <row r="16" spans="1:18" s="2" customFormat="1" ht="45">
+      <c r="A16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B16" s="4">
         <v>10.36</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C16" s="4">
         <v>4.34</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D16" s="4">
         <v>2.17</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="105">
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2" t="s">
+    <row r="19" spans="1:14" ht="105">
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="N19" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="3" t="s">
+    <row r="20" spans="1:14">
+      <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="6" t="s">
+    <row r="21" spans="1:14">
+      <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B21" s="4">
         <v>4.59</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" ht="30">
-      <c r="A20" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4">
-        <v>4.2300000000000004</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:14" ht="45">
-      <c r="A21" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="31" spans="1:14" ht="90">
-      <c r="A31" s="7" t="s">
+    <row r="22" spans="1:14" ht="30">
+      <c r="A22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:14" ht="45">
+      <c r="A23" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="33" spans="1:4" ht="90">
+      <c r="A33" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="5"/>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="3" t="s">
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="5"/>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="6" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B36" s="4">
         <v>9.9499999999999993</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C36" s="4">
         <v>3.51</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D36" s="4">
         <v>1.35</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30">
-      <c r="A35" s="6" t="s">
+    <row r="37" spans="1:4" ht="30">
+      <c r="A37" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B37" s="4">
         <v>11.07</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C37" s="4">
         <v>3.92</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D37" s="4">
         <v>1.49</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="45">
-      <c r="A36" s="6" t="s">
+    <row r="38" spans="1:4" ht="45">
+      <c r="A38" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="3" t="s">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="6" t="s">
+    <row r="43" spans="1:4">
+      <c r="A43" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B43" s="4">
         <v>3.9</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C43" s="4">
         <v>2.1</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D43" s="4">
         <v>1.23</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30">
-      <c r="A42" s="6" t="s">
+    <row r="44" spans="1:4" ht="30">
+      <c r="A44" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B44" s="4">
         <v>3.32</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C44" s="4">
         <v>1.78</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D44" s="4">
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="45">
-      <c r="A43" s="6" t="s">
+    <row r="45" spans="1:4" ht="45">
+      <c r="A45" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B45" s="4">
         <v>3.2</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C45" s="4">
         <v>1.54</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D45" s="4">
         <v>1.06</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2476,6 +2564,7 @@
     <mergeCell ref="N1:R1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Removed 'Model' attribute from Camera2.csv; now each camera unambiguously has 9 attributes Modified evaluationWithNominal.py, now there is no q1,q3,q5; but all queries are pre-generated in 'queries.txt' and read from the file generateTestCases.py generates queries into query.txt Added the option 'targetDoesntAppearInFirstCycle' in recommender.py
</commit_message>
<xml_diff>
--- a/src/Results.xlsx
+++ b/src/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>limitations:</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>similarProductsIn FirstCycle</t>
+  </si>
+  <si>
+    <t>q-1,3,5</t>
+  </si>
+  <si>
+    <t>In q-1,3,5 queries were read from text file queries.txt</t>
+  </si>
+  <si>
+    <t>Same queries were given to all methods when doing q-1,3,5</t>
+  </si>
+  <si>
+    <t>In real life scenarios, we expect the number of interaction cycles to be lesser; the target product may show up in the first iteration itself.</t>
   </si>
 </sst>
 </file>
@@ -255,18 +267,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -378,7 +390,7 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q5</c:v>
+                  <c:v>q-1,3,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -396,7 +408,7 @@
                   <c:v>4.82</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.21</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -429,7 +441,7 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q5</c:v>
+                  <c:v>q-1,3,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -445,9 +457,6 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.92</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -480,7 +489,7 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q5</c:v>
+                  <c:v>q-1,3,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -496,9 +505,6 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.84</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -531,7 +537,7 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q5</c:v>
+                  <c:v>q-1,3,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -545,11 +551,8 @@
                 <c:pt idx="0">
                   <c:v>6.56</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                <c:pt idx="2">
+                  <c:v>8.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -582,7 +585,7 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q5</c:v>
+                  <c:v>q-1,3,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -595,12 +598,6 @@
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>9.12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -633,7 +630,7 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q5</c:v>
+                  <c:v>q-1,3,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -678,7 +675,7 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q5</c:v>
+                  <c:v>q-1,3,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -705,11 +702,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="562139640"/>
-        <c:axId val="562128152"/>
+        <c:axId val="522944008"/>
+        <c:axId val="522946888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="562139640"/>
+        <c:axId val="522944008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -718,7 +715,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562128152"/>
+        <c:crossAx val="522946888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -726,7 +723,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="562128152"/>
+        <c:axId val="522946888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,7 +734,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562139640"/>
+        <c:crossAx val="522944008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -942,11 +939,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="579919160"/>
-        <c:axId val="579922136"/>
+        <c:axId val="523006600"/>
+        <c:axId val="523009576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="579919160"/>
+        <c:axId val="523006600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,7 +952,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="579922136"/>
+        <c:crossAx val="523009576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -963,7 +960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="579922136"/>
+        <c:axId val="523009576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -974,7 +971,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="579919160"/>
+        <c:crossAx val="523006600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1170,11 +1167,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="579952792"/>
-        <c:axId val="579955768"/>
+        <c:axId val="523040200"/>
+        <c:axId val="523043176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="579952792"/>
+        <c:axId val="523040200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1183,7 +1180,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="579955768"/>
+        <c:crossAx val="523043176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1191,7 +1188,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="579955768"/>
+        <c:axId val="523043176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1202,14 +1199,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="579952792"/>
+        <c:crossAx val="523040200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1407,11 +1403,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="579986696"/>
-        <c:axId val="579989672"/>
+        <c:axId val="523074424"/>
+        <c:axId val="523077400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="579986696"/>
+        <c:axId val="523074424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1420,7 +1416,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="579989672"/>
+        <c:crossAx val="523077400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1428,7 +1424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="579989672"/>
+        <c:axId val="523077400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1439,14 +1435,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="579986696"/>
+        <c:crossAx val="523074424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1623,11 +1618,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="580021336"/>
-        <c:axId val="580024312"/>
+        <c:axId val="523108856"/>
+        <c:axId val="523111832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="580021336"/>
+        <c:axId val="523108856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,7 +1631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="580024312"/>
+        <c:crossAx val="523111832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1644,7 +1639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="580024312"/>
+        <c:axId val="523111832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1655,14 +1650,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="580021336"/>
+        <c:crossAx val="523108856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2157,7 +2151,7 @@
   <dimension ref="A1:R48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2171,14 +2165,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="36" customHeight="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2188,13 +2182,13 @@
       <c r="M1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
@@ -2207,7 +2201,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2231,7 +2225,7 @@
         <v>4.82</v>
       </c>
       <c r="D3" s="4">
-        <v>2.21</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="35" customHeight="1">
@@ -2244,9 +2238,7 @@
       <c r="C4" s="4">
         <v>4.92</v>
       </c>
-      <c r="D4" s="4">
-        <v>2.57</v>
-      </c>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:18" ht="45">
       <c r="A5" s="6" t="s">
@@ -2258,43 +2250,35 @@
       <c r="C5" s="4">
         <v>4.84</v>
       </c>
-      <c r="D5" s="4">
-        <v>2.42</v>
-      </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:18" ht="30">
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="8">
         <v>6.56</v>
       </c>
-      <c r="C6" s="10">
-        <v>0</v>
-      </c>
-      <c r="D6" s="10">
-        <v>0</v>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
+        <v>8.56</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="30">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="8">
         <v>9.1199999999999992</v>
       </c>
-      <c r="C7" s="10">
-        <v>0</v>
-      </c>
-      <c r="D7" s="10">
-        <v>0</v>
-      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:18" ht="30">
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>3.37</v>
       </c>
       <c r="C8" s="4"/>
@@ -2304,17 +2288,28 @@
       <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="8">
         <v>2.15</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="3" t="s">
@@ -2564,7 +2559,6 @@
     <mergeCell ref="N1:R1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
evaluationWithNominal.py changed to evaluation.py Added a printNotes() function in util.py
</commit_message>
<xml_diff>
--- a/src/Results.xlsx
+++ b/src/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>limitations:</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>In real life scenarios, we expect the number of interaction cycles to be lesser; the target product may show up in the first iteration itself.</t>
+  </si>
+  <si>
+    <t>similarProdInFirstcycle+updateWeightsWrtInitialPreferences</t>
+  </si>
+  <si>
+    <t>similarProdInFirstcycle</t>
+  </si>
+  <si>
+    <t>Diverse critiques</t>
   </si>
 </sst>
 </file>
@@ -148,12 +157,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -189,7 +210,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -245,8 +266,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -268,19 +297,20 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -308,6 +338,10 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -335,6 +369,10 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -404,11 +442,8 @@
                 <c:pt idx="0">
                   <c:v>12.24</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.82</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14.4</c:v>
+                <c:pt idx="2">
+                  <c:v>14.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,10 +488,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.92</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -471,7 +503,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DiverseCritiquesWithSelectiveWtUpdate</c:v>
+                  <c:v>Diverse critiques</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -501,10 +533,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12.02</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.84</c:v>
+                  <c:v>9.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -549,10 +578,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.56</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.56</c:v>
+                  <c:v>7.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -599,6 +628,9 @@
                 <c:pt idx="0">
                   <c:v>9.12</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.94</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -612,7 +644,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>attributesInLineWithTarget</c:v>
+                  <c:v>similarProdInFirstcycle+updateWeightsWrtInitialPreferences</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -642,52 +674,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.37</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>allAttributesTowardsTarget</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>q1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>q3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>q-1,3,5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$9:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2.15</c:v>
+                  <c:v>6.86</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -702,11 +692,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="522944008"/>
-        <c:axId val="522946888"/>
+        <c:axId val="643945848"/>
+        <c:axId val="643948728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="522944008"/>
+        <c:axId val="643945848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -715,7 +705,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="522946888"/>
+        <c:crossAx val="643948728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -723,7 +713,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="522946888"/>
+        <c:axId val="643948728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -734,7 +724,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="522944008"/>
+        <c:crossAx val="643945848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -816,13 +806,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10.37</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.52</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.27</c:v>
+                  <c:v>6.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -867,13 +851,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10.3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.02</c:v>
+                  <c:v>8.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -888,7 +866,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DiverseCritiquesWithSelectiveWtUpdate</c:v>
+                  <c:v>Diverse critiques</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -918,13 +896,142 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10.36</c:v>
+                  <c:v>5.52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>similarProdInFirstcycle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.34</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.17</c:v>
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>updateWeightsWrtInitialPreferences</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>similarProdInFirstcycle+updateWeightsWrtInitialPreferences</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$19:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -939,11 +1046,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="523006600"/>
-        <c:axId val="523009576"/>
+        <c:axId val="644026856"/>
+        <c:axId val="644029832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="523006600"/>
+        <c:axId val="644026856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -952,7 +1059,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523009576"/>
+        <c:crossAx val="644029832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -960,7 +1067,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523009576"/>
+        <c:axId val="644029832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,7 +1078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523006600"/>
+        <c:crossAx val="644026856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1019,7 +1126,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$36</c:f>
+              <c:f>Sheet1!$A$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1031,7 +1138,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$35:$D$35</c:f>
+              <c:f>Sheet1!$B$41:$D$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1048,7 +1155,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$36:$D$36</c:f>
+              <c:f>Sheet1!$B$42:$D$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1070,7 +1177,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$37</c:f>
+              <c:f>Sheet1!$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1082,7 +1189,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$35:$D$35</c:f>
+              <c:f>Sheet1!$B$41:$D$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1099,7 +1206,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$37:$D$37</c:f>
+              <c:f>Sheet1!$B$43:$D$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1121,7 +1228,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$38</c:f>
+              <c:f>Sheet1!$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1133,7 +1240,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$35:$D$35</c:f>
+              <c:f>Sheet1!$B$41:$D$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1150,7 +1257,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$38:$D$38</c:f>
+              <c:f>Sheet1!$B$44:$D$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1167,11 +1274,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="523040200"/>
-        <c:axId val="523043176"/>
+        <c:axId val="644060424"/>
+        <c:axId val="644063400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="523040200"/>
+        <c:axId val="644060424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,7 +1287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523043176"/>
+        <c:crossAx val="644063400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1188,7 +1295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523043176"/>
+        <c:axId val="644063400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,13 +1306,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523040200"/>
+        <c:crossAx val="644060424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1246,7 +1354,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$43</c:f>
+              <c:f>Sheet1!$A$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1258,7 +1366,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$42:$D$42</c:f>
+              <c:f>Sheet1!$B$48:$D$48</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1275,7 +1383,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$D$43</c:f>
+              <c:f>Sheet1!$B$49:$D$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1297,7 +1405,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$44</c:f>
+              <c:f>Sheet1!$A$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1309,7 +1417,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$42:$D$42</c:f>
+              <c:f>Sheet1!$B$48:$D$48</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1326,7 +1434,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$44:$D$44</c:f>
+              <c:f>Sheet1!$B$50:$D$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1348,7 +1456,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$45</c:f>
+              <c:f>Sheet1!$A$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1360,7 +1468,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$42:$D$42</c:f>
+              <c:f>Sheet1!$B$48:$D$48</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1377,7 +1485,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$45:$D$45</c:f>
+              <c:f>Sheet1!$B$51:$D$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1403,11 +1511,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="523074424"/>
-        <c:axId val="523077400"/>
+        <c:axId val="644094648"/>
+        <c:axId val="644097624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="523074424"/>
+        <c:axId val="644094648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1416,7 +1524,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523077400"/>
+        <c:crossAx val="644097624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1424,7 +1532,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523077400"/>
+        <c:axId val="644097624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1435,13 +1543,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523074424"/>
+        <c:crossAx val="644094648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1482,7 +1591,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$21</c:f>
+              <c:f>Sheet1!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1494,7 +1603,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$20:$D$20</c:f>
+              <c:f>Sheet1!$B$26:$D$26</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1511,7 +1620,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$21:$D$21</c:f>
+              <c:f>Sheet1!$B$27:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1527,7 +1636,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$22</c:f>
+              <c:f>Sheet1!$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1539,7 +1648,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$20:$D$20</c:f>
+              <c:f>Sheet1!$B$26:$D$26</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1556,7 +1665,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$22:$D$22</c:f>
+              <c:f>Sheet1!$B$28:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1572,7 +1681,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$23</c:f>
+              <c:f>Sheet1!$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1584,7 +1693,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$20:$D$20</c:f>
+              <c:f>Sheet1!$B$26:$D$26</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1601,7 +1710,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$23:$D$23</c:f>
+              <c:f>Sheet1!$B$29:$D$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1618,11 +1727,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="523108856"/>
-        <c:axId val="523111832"/>
+        <c:axId val="644129368"/>
+        <c:axId val="644132344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="523108856"/>
+        <c:axId val="644129368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1631,7 +1740,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523111832"/>
+        <c:crossAx val="644132344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1639,7 +1748,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523111832"/>
+        <c:axId val="644132344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,13 +1759,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523108856"/>
+        <c:crossAx val="644129368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1682,9 +1792,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2478688</xdr:colOff>
+      <xdr:colOff>2461172</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>175171</xdr:rowOff>
+      <xdr:rowOff>359103</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1706,15 +1816,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>420413</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>122614</xdr:rowOff>
+      <xdr:colOff>490483</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>105104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2417378</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>157655</xdr:rowOff>
+      <xdr:colOff>2522482</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1737,13 +1847,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>613103</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>116928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2312276</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>131380</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1767,13 +1877,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>604344</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>122621</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2338551</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>183931</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1796,15 +1906,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>437930</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>832069</xdr:rowOff>
+      <xdr:colOff>376620</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>52552</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2601309</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>149771</xdr:rowOff>
+      <xdr:colOff>2539999</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>123495</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2148,10 +2258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2165,14 +2275,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="36" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2182,13 +2292,13 @@
       <c r="M1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
@@ -2215,74 +2325,72 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="4">
         <v>12.24</v>
       </c>
-      <c r="C3" s="4">
-        <v>4.82</v>
-      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="4">
-        <v>14.4</v>
+        <v>14.54</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="35" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="4">
-        <v>12.2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>4.92</v>
-      </c>
+        <v>12.8</v>
+      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="45">
-      <c r="A5" s="6" t="s">
-        <v>17</v>
+    <row r="5" spans="1:18">
+      <c r="A5" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="B5" s="4">
-        <v>12.02</v>
-      </c>
-      <c r="C5" s="4">
-        <v>4.84</v>
-      </c>
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:18" ht="30">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="8">
-        <v>6.56</v>
+        <v>7.18</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8">
-        <v>8.56</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="30">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="8">
         <v>9.1199999999999992</v>
       </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:18" ht="30">
-      <c r="A8" s="6" t="s">
-        <v>23</v>
+      <c r="D7" s="8">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="60">
+      <c r="A8" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="B8" s="8">
-        <v>3.37</v>
+        <v>6.86</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4">
+        <v>6.11</v>
+      </c>
     </row>
     <row r="9" spans="1:18" ht="30">
       <c r="A9" s="6" t="s">
@@ -2297,11 +2405,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+    <row r="10" spans="1:18" ht="30" customHeight="1">
+      <c r="A10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="8">
+        <v>3.37</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
       <c r="F10" t="s">
         <v>28</v>
       </c>
@@ -2330,44 +2442,60 @@
         <v>18</v>
       </c>
       <c r="B14" s="4">
-        <v>10.37</v>
-      </c>
-      <c r="C14" s="4">
-        <v>4.5199999999999996</v>
-      </c>
-      <c r="D14" s="4">
-        <v>2.27</v>
-      </c>
+        <v>6.79</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:18" ht="30">
       <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="4">
-        <v>10.3</v>
-      </c>
-      <c r="C15" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="D15" s="4">
-        <v>2.02</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" s="2" customFormat="1" ht="45">
+        <v>8.18</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" s="2" customFormat="1">
       <c r="A16" s="6" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B16" s="4">
-        <v>10.36</v>
-      </c>
-      <c r="C16" s="4">
-        <v>4.34</v>
-      </c>
-      <c r="D16" s="4">
-        <v>2.17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="105">
+        <v>5.52</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" ht="30">
+      <c r="A17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="8">
+        <v>4.57</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:14" ht="30">
+      <c r="A18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="8">
+        <v>5.64</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" ht="48" customHeight="1">
+      <c r="A19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="8">
+        <v>3.92</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2" t="s">
@@ -2383,175 +2511,175 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="3" t="s">
+    <row r="26" spans="1:14">
+      <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="6" t="s">
+    <row r="27" spans="1:14">
+      <c r="A27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B27" s="4">
         <v>4.59</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:14" ht="30">
-      <c r="A22" s="6" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" ht="30">
+      <c r="A28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B28" s="4">
         <v>4.2300000000000004</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:14" ht="45">
-      <c r="A23" s="6" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:14" ht="45">
+      <c r="A29" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="33" spans="1:4" ht="90">
-      <c r="A33" s="7" t="s">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="39" spans="1:4" ht="90">
+      <c r="A39" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="5"/>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="3" t="s">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="5"/>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="6" t="s">
+    <row r="42" spans="1:4">
+      <c r="A42" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B42" s="4">
         <v>9.9499999999999993</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C42" s="4">
         <v>3.51</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D42" s="4">
         <v>1.35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30">
-      <c r="A37" s="6" t="s">
+    <row r="43" spans="1:4" ht="30">
+      <c r="A43" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B43" s="4">
         <v>11.07</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C43" s="4">
         <v>3.92</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D43" s="4">
         <v>1.49</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="45">
-      <c r="A38" s="6" t="s">
+    <row r="44" spans="1:4" ht="45">
+      <c r="A44" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="4">
-        <v>3.9</v>
-      </c>
-      <c r="C43" s="4">
-        <v>2.1</v>
-      </c>
-      <c r="D43" s="4">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30">
-      <c r="A44" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="4">
-        <v>3.32</v>
-      </c>
-      <c r="C44" s="4">
-        <v>1.78</v>
-      </c>
-      <c r="D44" s="4">
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="45">
-      <c r="A45" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="C45" s="4">
-        <v>1.54</v>
-      </c>
-      <c r="D45" s="4">
-        <v>1.06</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48"/>
+      <c r="A48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="C49" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="D49" s="4">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30">
+      <c r="A50" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="4">
+        <v>3.32</v>
+      </c>
+      <c r="C50" s="4">
+        <v>1.78</v>
+      </c>
+      <c r="D50" s="4">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="45">
+      <c r="A51" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="C51" s="4">
+        <v>1.54</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2559,6 +2687,7 @@
     <mergeCell ref="N1:R1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Created dictionaries maxV, minV which precompute max and min values of numeric attributes respectively.
</commit_message>
<xml_diff>
--- a/src/Results.xlsx
+++ b/src/Results.xlsx
@@ -626,7 +626,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9.12</c:v>
+                  <c:v>8.62</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6.94</c:v>
@@ -1786,15 +1786,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>394137</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>148895</xdr:rowOff>
+      <xdr:colOff>630619</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>166413</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2461172</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>359103</xdr:rowOff>
+      <xdr:colOff>2697654</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>70069</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2260,8 +2260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2373,7 +2373,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="8">
-        <v>9.1199999999999992</v>
+        <v>8.6199999999999992</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8">
@@ -2438,7 +2438,7 @@
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="4">
@@ -2448,7 +2448,7 @@
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:18" ht="30">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="4">
@@ -2458,7 +2458,7 @@
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:18" s="2" customFormat="1">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="4">
@@ -2468,7 +2468,7 @@
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:14" ht="30">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="8">
@@ -2478,7 +2478,7 @@
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:14" ht="30">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="8">
@@ -2488,7 +2488,7 @@
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:14" ht="48" customHeight="1">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="8">

</xml_diff>

<commit_message>
Added the 'averageProductEnabled' option. Working completely fine... weights2 and weights3 folders contain graphs that depict variation of weights for a single product during a single experiment.
</commit_message>
<xml_diff>
--- a/src/Results.xlsx
+++ b/src/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>limitations:</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Diverse critiques</t>
+  </si>
+  <si>
+    <t>averagingSelectedProduct</t>
   </si>
 </sst>
 </file>
@@ -297,17 +300,17 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="63">
@@ -692,11 +695,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="643945848"/>
-        <c:axId val="643948728"/>
+        <c:axId val="547897272"/>
+        <c:axId val="547900536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="643945848"/>
+        <c:axId val="547897272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,7 +708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="643948728"/>
+        <c:crossAx val="547900536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -713,7 +716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="643948728"/>
+        <c:axId val="547900536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -724,7 +727,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="643945848"/>
+        <c:crossAx val="547897272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -772,7 +775,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$14</c:f>
+              <c:f>Sheet1!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -784,7 +787,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:f>Sheet1!$B$16:$D$16</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -801,7 +804,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$D$14</c:f>
+              <c:f>Sheet1!$B$17:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -817,7 +820,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
+              <c:f>Sheet1!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -829,7 +832,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:f>Sheet1!$B$16:$D$16</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -846,7 +849,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$D$15</c:f>
+              <c:f>Sheet1!$B$18:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -862,7 +865,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$16</c:f>
+              <c:f>Sheet1!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -874,7 +877,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:f>Sheet1!$B$16:$D$16</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -891,7 +894,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$D$16</c:f>
+              <c:f>Sheet1!$B$19:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -907,7 +910,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$17</c:f>
+              <c:f>Sheet1!$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -919,7 +922,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:f>Sheet1!$B$16:$D$16</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -936,7 +939,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$D$17</c:f>
+              <c:f>Sheet1!$B$20:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -952,7 +955,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$18</c:f>
+              <c:f>Sheet1!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -964,7 +967,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:f>Sheet1!$B$16:$D$16</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -981,7 +984,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$18:$D$18</c:f>
+              <c:f>Sheet1!$B$21:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -997,7 +1000,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$19</c:f>
+              <c:f>Sheet1!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1009,7 +1012,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:f>Sheet1!$B$16:$D$16</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1026,7 +1029,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$D$19</c:f>
+              <c:f>Sheet1!$B$22:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1046,11 +1049,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="644026856"/>
-        <c:axId val="644029832"/>
+        <c:axId val="547991880"/>
+        <c:axId val="547995016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="644026856"/>
+        <c:axId val="547991880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1059,7 +1062,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="644029832"/>
+        <c:crossAx val="547995016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1067,7 +1070,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="644029832"/>
+        <c:axId val="547995016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1081,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="644026856"/>
+        <c:crossAx val="547991880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1126,7 +1129,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$42</c:f>
+              <c:f>Sheet1!$A$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1138,7 +1141,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$41:$D$41</c:f>
+              <c:f>Sheet1!$B$44:$D$44</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1155,7 +1158,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$42:$D$42</c:f>
+              <c:f>Sheet1!$B$45:$D$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1177,7 +1180,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$43</c:f>
+              <c:f>Sheet1!$A$46</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1189,7 +1192,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$41:$D$41</c:f>
+              <c:f>Sheet1!$B$44:$D$44</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1206,7 +1209,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$D$43</c:f>
+              <c:f>Sheet1!$B$46:$D$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1228,7 +1231,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$44</c:f>
+              <c:f>Sheet1!$A$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1240,7 +1243,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$41:$D$41</c:f>
+              <c:f>Sheet1!$B$44:$D$44</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1257,7 +1260,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$44:$D$44</c:f>
+              <c:f>Sheet1!$B$47:$D$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1274,11 +1277,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="644060424"/>
-        <c:axId val="644063400"/>
+        <c:axId val="548022888"/>
+        <c:axId val="548025864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="644060424"/>
+        <c:axId val="548022888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1287,7 +1290,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="644063400"/>
+        <c:crossAx val="548025864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1295,7 +1298,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="644063400"/>
+        <c:axId val="548025864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1306,14 +1309,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="644060424"/>
+        <c:crossAx val="548022888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1354,7 +1356,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$49</c:f>
+              <c:f>Sheet1!$A$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1366,7 +1368,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$48:$D$48</c:f>
+              <c:f>Sheet1!$B$51:$D$51</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1383,7 +1385,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$49:$D$49</c:f>
+              <c:f>Sheet1!$B$52:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1405,7 +1407,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$50</c:f>
+              <c:f>Sheet1!$A$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1417,7 +1419,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$48:$D$48</c:f>
+              <c:f>Sheet1!$B$51:$D$51</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1434,7 +1436,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$50:$D$50</c:f>
+              <c:f>Sheet1!$B$53:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1456,7 +1458,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$51</c:f>
+              <c:f>Sheet1!$A$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1468,7 +1470,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$48:$D$48</c:f>
+              <c:f>Sheet1!$B$51:$D$51</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1485,7 +1487,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$51:$D$51</c:f>
+              <c:f>Sheet1!$B$54:$D$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1511,11 +1513,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="644094648"/>
-        <c:axId val="644097624"/>
+        <c:axId val="548057512"/>
+        <c:axId val="548060488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="644094648"/>
+        <c:axId val="548057512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1524,7 +1526,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="644097624"/>
+        <c:crossAx val="548060488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1532,7 +1534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="644097624"/>
+        <c:axId val="548060488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1543,14 +1545,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="644094648"/>
+        <c:crossAx val="548057512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1591,7 +1592,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$27</c:f>
+              <c:f>Sheet1!$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1603,7 +1604,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$26:$D$26</c:f>
+              <c:f>Sheet1!$B$29:$D$29</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1620,7 +1621,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$27:$D$27</c:f>
+              <c:f>Sheet1!$B$30:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1636,7 +1637,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$28</c:f>
+              <c:f>Sheet1!$A$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1648,7 +1649,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$26:$D$26</c:f>
+              <c:f>Sheet1!$B$29:$D$29</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1665,7 +1666,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$28:$D$28</c:f>
+              <c:f>Sheet1!$B$31:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1681,7 +1682,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$29</c:f>
+              <c:f>Sheet1!$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1693,7 +1694,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$26:$D$26</c:f>
+              <c:f>Sheet1!$B$29:$D$29</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1710,7 +1711,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$29:$D$29</c:f>
+              <c:f>Sheet1!$B$32:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1727,11 +1728,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="644129368"/>
-        <c:axId val="644132344"/>
+        <c:axId val="548092504"/>
+        <c:axId val="548095480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="644129368"/>
+        <c:axId val="548092504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1740,7 +1741,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="644132344"/>
+        <c:crossAx val="548095480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1748,7 +1749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="644132344"/>
+        <c:axId val="548095480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1759,14 +1760,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="644129368"/>
+        <c:crossAx val="548092504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1817,13 +1817,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>490483</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>105104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2522482</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>26276</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1847,13 +1847,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>613103</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>116928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2312276</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>131380</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1877,13 +1877,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>604344</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>122621</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2338551</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>183931</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1907,13 +1907,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>376620</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>52552</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2539999</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>123495</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2258,10 +2258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R54"/>
+  <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2275,14 +2275,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="36" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2292,13 +2292,13 @@
       <c r="M1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
@@ -2325,7 +2325,7 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="4">
@@ -2337,7 +2337,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="35" customHeight="1">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="4">
@@ -2347,7 +2347,7 @@
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="4">
@@ -2357,7 +2357,7 @@
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:18" ht="30">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="8">
@@ -2369,7 +2369,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="30">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="8">
@@ -2381,7 +2381,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="60">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="8">
@@ -2406,7 +2406,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" ht="30" customHeight="1">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="8">
@@ -2418,268 +2418,276 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" ht="30">
+      <c r="A11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="4">
+        <v>11.34</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
       <c r="F11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="3" t="s">
+    <row r="16" spans="1:18">
+      <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="11" t="s">
+    <row r="17" spans="1:14">
+      <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B17" s="4">
         <v>6.79</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:18" ht="30">
-      <c r="A15" s="11" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:14" ht="30">
+      <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B18" s="4">
         <v>8.18</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:18" s="2" customFormat="1">
-      <c r="A16" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="4">
-        <v>5.52</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:14" ht="30">
-      <c r="A17" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="8">
-        <v>4.57</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:14" ht="30">
-      <c r="A18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="8">
-        <v>5.64</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:14" ht="48" customHeight="1">
-      <c r="A19" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="8">
-        <v>3.92</v>
+    <row r="19" spans="1:14" s="2" customFormat="1">
+      <c r="A19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="4">
+        <v>5.52</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:14" ht="30">
+      <c r="A20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="8">
+        <v>4.57</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" ht="30">
+      <c r="A21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="8">
+        <v>5.64</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:14" ht="48" customHeight="1">
+      <c r="A22" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="8">
+        <v>3.92</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="N22" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="3" t="s">
+    <row r="29" spans="1:14">
+      <c r="A29" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="6" t="s">
+    <row r="30" spans="1:14">
+      <c r="A30" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B30" s="4">
         <v>4.59</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:14" ht="30">
-      <c r="A28" s="6" t="s">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" ht="30">
+      <c r="A31" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B31" s="4">
         <v>4.2300000000000004</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:14" ht="45">
-      <c r="A29" s="6" t="s">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:14" ht="45">
+      <c r="A32" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="39" spans="1:4" ht="90">
-      <c r="A39" s="7" t="s">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="42" spans="1:4" ht="90">
+      <c r="A42" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="5"/>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="3" t="s">
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="5"/>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="6" t="s">
+    <row r="45" spans="1:4">
+      <c r="A45" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B45" s="4">
         <v>9.9499999999999993</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C45" s="4">
         <v>3.51</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D45" s="4">
         <v>1.35</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30">
-      <c r="A43" s="6" t="s">
+    <row r="46" spans="1:4" ht="30">
+      <c r="A46" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B46" s="4">
         <v>11.07</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C46" s="4">
         <v>3.92</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D46" s="4">
         <v>1.49</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="45">
-      <c r="A44" s="6" t="s">
+    <row r="47" spans="1:4" ht="45">
+      <c r="A47" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="3" t="s">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="6" t="s">
+    <row r="52" spans="1:4">
+      <c r="A52" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B52" s="4">
         <v>3.9</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C52" s="4">
         <v>2.1</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D52" s="4">
         <v>1.23</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30">
-      <c r="A50" s="6" t="s">
+    <row r="53" spans="1:4" ht="30">
+      <c r="A53" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B53" s="4">
         <v>3.32</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C53" s="4">
         <v>1.78</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D53" s="4">
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="45">
-      <c r="A51" s="6" t="s">
+    <row r="54" spans="1:4" ht="45">
+      <c r="A54" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B54" s="4">
         <v>3.2</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C54" s="4">
         <v>1.54</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D54" s="4">
         <v>1.06</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54"/>
+    <row r="55" spans="1:4">
+      <c r="A55"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2687,7 +2695,6 @@
     <mergeCell ref="N1:R1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Added a new option 'deepHistoryEnabled'; that takes all reference and selected products seen till now into consideration;
</commit_message>
<xml_diff>
--- a/src/Results.xlsx
+++ b/src/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
     <t>limitations:</t>
   </si>
@@ -121,6 +121,30 @@
   </si>
   <si>
     <t>averagingSelectedProduct</t>
+  </si>
+  <si>
+    <t>Results for the presentation</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>DIV - diversity in every cycle</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>MOD</t>
+  </si>
+  <si>
+    <t>Additional term in utility function/ History</t>
+  </si>
+  <si>
+    <t>SimilarProdInFirstCycle</t>
+  </si>
+  <si>
+    <t>SIM</t>
   </si>
 </sst>
 </file>
@@ -213,8 +237,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -313,7 +349,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -345,6 +381,12 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -376,6 +418,12 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -695,11 +743,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="547897272"/>
-        <c:axId val="547900536"/>
+        <c:axId val="425836664"/>
+        <c:axId val="425839800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="547897272"/>
+        <c:axId val="425836664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -708,7 +756,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="547900536"/>
+        <c:crossAx val="425839800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -716,7 +764,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="547900536"/>
+        <c:axId val="425839800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -727,7 +775,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="547897272"/>
+        <c:crossAx val="425836664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1049,11 +1097,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="547991880"/>
-        <c:axId val="547995016"/>
+        <c:axId val="425913544"/>
+        <c:axId val="425916680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="547991880"/>
+        <c:axId val="425913544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1062,7 +1110,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="547995016"/>
+        <c:crossAx val="425916680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1070,7 +1118,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="547995016"/>
+        <c:axId val="425916680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1081,7 +1129,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="547991880"/>
+        <c:crossAx val="425913544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1277,11 +1325,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="548022888"/>
-        <c:axId val="548025864"/>
+        <c:axId val="425944392"/>
+        <c:axId val="425947368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="548022888"/>
+        <c:axId val="425944392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1290,7 +1338,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="548025864"/>
+        <c:crossAx val="425947368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1298,7 +1346,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="548025864"/>
+        <c:axId val="425947368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,13 +1357,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="548022888"/>
+        <c:crossAx val="425944392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1513,11 +1562,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="548057512"/>
-        <c:axId val="548060488"/>
+        <c:axId val="425979016"/>
+        <c:axId val="425981992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="548057512"/>
+        <c:axId val="425979016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1526,7 +1575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="548060488"/>
+        <c:crossAx val="425981992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1534,7 +1583,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="548060488"/>
+        <c:axId val="425981992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1545,13 +1594,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="548057512"/>
+        <c:crossAx val="425979016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1728,11 +1778,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="548092504"/>
-        <c:axId val="548095480"/>
+        <c:axId val="426013752"/>
+        <c:axId val="426016728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="548092504"/>
+        <c:axId val="426013752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1741,7 +1791,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="548095480"/>
+        <c:crossAx val="426016728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1749,7 +1799,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="548095480"/>
+        <c:axId val="426016728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1760,13 +1810,623 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="548092504"/>
+        <c:crossAx val="426013752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MAUT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$61:$D$61</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$62:$D$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$61:$D$61</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$63:$D$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DIV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$61:$D$61</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$64:$D$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="453884280"/>
+        <c:axId val="456141112"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="453884280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="456141112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="456141112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="453884280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$69</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MAUT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$68:$D$68</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$69:$D$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$70</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$68:$D$68</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$70:$D$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="454174488"/>
+        <c:axId val="435121480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="454174488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="435121480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="435121480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="454174488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$78</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MAUT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$77:$D$77</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$78:$D$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$79</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SIM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$77:$D$77</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$79:$D$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="434798200"/>
+        <c:axId val="462401432"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="434798200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="462401432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="462401432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="434798200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1928,6 +2588,96 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>814550</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>61310</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1103585</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>162910</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>26276</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>8757</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1287517</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>40287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>43791</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>105104</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1129861</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>171669</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2258,10 +3008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R57"/>
+  <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="A79" sqref="A77:D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2689,12 +3439,165 @@
     <row r="57" spans="1:4">
       <c r="A57"/>
     </row>
+    <row r="60" spans="1:4" ht="30">
+      <c r="A60" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="6"/>
+      <c r="B61" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" s="4">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="C62" s="4">
+        <v>3.91</v>
+      </c>
+      <c r="D62" s="4">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63" s="4">
+        <v>8.42</v>
+      </c>
+      <c r="C63" s="4">
+        <v>3.65</v>
+      </c>
+      <c r="D63" s="4">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B64" s="4">
+        <v>7.22</v>
+      </c>
+      <c r="C64" s="4">
+        <v>3.08</v>
+      </c>
+      <c r="D64" s="4">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="45">
+      <c r="A67" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="6"/>
+      <c r="B68" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" s="4">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="C69" s="4">
+        <v>3.91</v>
+      </c>
+      <c r="D69" s="4">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B70" s="4">
+        <v>7.23</v>
+      </c>
+      <c r="C70" s="4">
+        <v>2.95</v>
+      </c>
+      <c r="D70" s="4">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="30">
+      <c r="A76" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="6"/>
+      <c r="B77" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78" s="4">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="C78" s="4">
+        <v>3.91</v>
+      </c>
+      <c r="D78" s="4">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79" s="4">
+        <v>6.24</v>
+      </c>
+      <c r="C79" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D79" s="4">
+        <v>1.6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="N1:R1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
All the techniques working properly; with the results recorded almost accurately in Results.xslx The performance improvement will only be better than what is actually in Results.xlsx
</commit_message>
<xml_diff>
--- a/src/Results.xlsx
+++ b/src/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>limitations:</t>
   </si>
@@ -96,21 +96,6 @@
     <t>allAttributesTowardsTarget</t>
   </si>
   <si>
-    <t>similarProductsIn FirstCycle</t>
-  </si>
-  <si>
-    <t>q-1,3,5</t>
-  </si>
-  <si>
-    <t>In q-1,3,5 queries were read from text file queries.txt</t>
-  </si>
-  <si>
-    <t>Same queries were given to all methods when doing q-1,3,5</t>
-  </si>
-  <si>
-    <t>In real life scenarios, we expect the number of interaction cycles to be lesser; the target product may show up in the first iteration itself.</t>
-  </si>
-  <si>
     <t>similarProdInFirstcycle+updateWeightsWrtInitialPreferences</t>
   </si>
   <si>
@@ -145,6 +130,51 @@
   </si>
   <si>
     <t>SIM</t>
+  </si>
+  <si>
+    <t>MAUT-additive</t>
+  </si>
+  <si>
+    <t>Adaptive Selection</t>
+  </si>
+  <si>
+    <t>MAUT-paper</t>
+  </si>
+  <si>
+    <t>AdditionalPref to products satisfying critiques</t>
+  </si>
+  <si>
+    <t>wMLT for nominal attributes*</t>
+  </si>
+  <si>
+    <t>*with the best parameter \alpha = 0.5</t>
+  </si>
+  <si>
+    <t>Diverse Critiques in Every Cycle</t>
+  </si>
+  <si>
+    <t>Adaptive Selection with Neutral Updates</t>
+  </si>
+  <si>
+    <t>%impr</t>
+  </si>
+  <si>
+    <t>Similar Products in First Cycle</t>
+  </si>
+  <si>
+    <t>Neutral Updates Enabled</t>
+  </si>
+  <si>
+    <t>averageProduct Enabled</t>
+  </si>
+  <si>
+    <t>selectively updating weights of numeric attributes</t>
+  </si>
+  <si>
+    <t>updating attribute weights wrt initial preferences</t>
+  </si>
+  <si>
+    <t>penalizing long jumps(?)</t>
   </si>
 </sst>
 </file>
@@ -237,7 +267,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -313,8 +343,70 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -343,13 +435,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="137">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -387,6 +495,37 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -424,6 +563,37 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,7 +627,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet1!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -469,7 +639,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:f>Sheet1!$B$23:$D$23</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -479,22 +649,19 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q-1,3,5</c:v>
+                  <c:v>q5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$D$3</c:f>
+              <c:f>Sheet1!$B$24:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12.24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14.54</c:v>
+                  <c:v>6.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -505,7 +672,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>Sheet1!$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -517,7 +684,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:f>Sheet1!$B$23:$D$23</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -527,19 +694,19 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q-1,3,5</c:v>
+                  <c:v>q5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$D$4</c:f>
+              <c:f>Sheet1!$B$25:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12.8</c:v>
+                  <c:v>8.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -550,7 +717,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>Sheet1!$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -562,7 +729,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:f>Sheet1!$B$23:$D$23</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -572,19 +739,19 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q-1,3,5</c:v>
+                  <c:v>q5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$D$5</c:f>
+              <c:f>Sheet1!$B$26:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9.12</c:v>
+                  <c:v>5.52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,11 +762,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$6</c:f>
+              <c:f>Sheet1!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>similarProductsIn FirstCycle</c:v>
+                  <c:v>similarProdInFirstcycle</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -607,7 +774,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:f>Sheet1!$B$23:$D$23</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -617,22 +784,19 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q-1,3,5</c:v>
+                  <c:v>q5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$D$6</c:f>
+              <c:f>Sheet1!$B$27:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.1</c:v>
+                  <c:v>4.57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -643,7 +807,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
+              <c:f>Sheet1!$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -655,7 +819,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:f>Sheet1!$B$23:$D$23</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -665,22 +829,19 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q-1,3,5</c:v>
+                  <c:v>q5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$D$7</c:f>
+              <c:f>Sheet1!$B$28:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.62</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.94</c:v>
+                  <c:v>5.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -691,7 +852,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
+              <c:f>Sheet1!$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -703,7 +864,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:f>Sheet1!$B$23:$D$23</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -713,22 +874,19 @@
                   <c:v>q3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>q-1,3,5</c:v>
+                  <c:v>q5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$D$8</c:f>
+              <c:f>Sheet1!$B$29:$D$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.86</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.11</c:v>
+                  <c:v>3.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -743,11 +901,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="425836664"/>
-        <c:axId val="425839800"/>
+        <c:axId val="474518328"/>
+        <c:axId val="474521624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="425836664"/>
+        <c:axId val="474518328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -756,7 +914,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425839800"/>
+        <c:crossAx val="474521624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -764,7 +922,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425839800"/>
+        <c:axId val="474521624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,7 +933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425836664"/>
+        <c:crossAx val="474518328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -823,7 +981,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$17</c:f>
+              <c:f>Sheet1!$A$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -835,7 +993,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$16:$D$16</c:f>
+              <c:f>Sheet1!$B$51:$D$51</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -852,12 +1010,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$D$17</c:f>
+              <c:f>Sheet1!$B$52:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.79</c:v>
+                  <c:v>9.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -868,7 +1032,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$18</c:f>
+              <c:f>Sheet1!$A$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -880,7 +1044,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$16:$D$16</c:f>
+              <c:f>Sheet1!$B$51:$D$51</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -897,12 +1061,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$18:$D$18</c:f>
+              <c:f>Sheet1!$B$53:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.18</c:v>
+                  <c:v>11.07</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -913,11 +1083,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$19</c:f>
+              <c:f>Sheet1!$A$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Diverse critiques</c:v>
+                  <c:v>DiverseCritiquesWithSelectiveWtUpdate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -925,7 +1095,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$16:$D$16</c:f>
+              <c:f>Sheet1!$B$51:$D$51</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -942,148 +1112,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$D$19</c:f>
+              <c:f>Sheet1!$B$54:$D$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>5.52</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>similarProdInFirstcycle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$16:$D$16</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>q1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>q3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>q5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$20:$D$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>4.57</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$21</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>updateWeightsWrtInitialPreferences</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$16:$D$16</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>q1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>q3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>q5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$21:$D$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>5.64</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>similarProdInFirstcycle+updateWeightsWrtInitialPreferences</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$16:$D$16</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>q1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>q3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>q5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$22:$D$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>3.92</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1097,11 +1129,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="425913544"/>
-        <c:axId val="425916680"/>
+        <c:axId val="474599960"/>
+        <c:axId val="474602936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="425913544"/>
+        <c:axId val="474599960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,7 +1142,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425916680"/>
+        <c:crossAx val="474602936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1118,7 +1150,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425916680"/>
+        <c:axId val="474602936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,7 +1161,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425913544"/>
+        <c:crossAx val="474599960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1177,7 +1209,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$45</c:f>
+              <c:f>Sheet1!$A$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1189,7 +1221,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$44:$D$44</c:f>
+              <c:f>Sheet1!$B$58:$D$58</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1206,18 +1238,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$45:$D$45</c:f>
+              <c:f>Sheet1!$B$59:$D$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9.95</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.51</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.35</c:v>
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1228,7 +1260,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$46</c:f>
+              <c:f>Sheet1!$A$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1240,7 +1272,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$44:$D$44</c:f>
+              <c:f>Sheet1!$B$58:$D$58</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1257,18 +1289,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$46:$D$46</c:f>
+              <c:f>Sheet1!$B$60:$D$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>11.07</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.92</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.49</c:v>
+                  <c:v>3.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1279,7 +1311,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$47</c:f>
+              <c:f>Sheet1!$A$61</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1291,7 +1323,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$44:$D$44</c:f>
+              <c:f>Sheet1!$B$58:$D$58</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1308,10 +1340,19 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$47:$D$47</c:f>
+              <c:f>Sheet1!$B$61:$D$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.06</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1325,11 +1366,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="425944392"/>
-        <c:axId val="425947368"/>
+        <c:axId val="474633960"/>
+        <c:axId val="474636936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="425944392"/>
+        <c:axId val="474633960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,7 +1379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425947368"/>
+        <c:crossAx val="474636936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1346,7 +1387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425947368"/>
+        <c:axId val="474636936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1357,7 +1398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425944392"/>
+        <c:crossAx val="474633960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1405,7 +1446,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$52</c:f>
+              <c:f>Sheet1!$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1417,7 +1458,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$51:$D$51</c:f>
+              <c:f>Sheet1!$B$36:$D$36</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1434,18 +1475,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$52:$D$52</c:f>
+              <c:f>Sheet1!$B$37:$D$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.23</c:v>
+                  <c:v>4.59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1456,7 +1491,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$53</c:f>
+              <c:f>Sheet1!$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1468,7 +1503,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$51:$D$51</c:f>
+              <c:f>Sheet1!$B$36:$D$36</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1485,18 +1520,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$53:$D$53</c:f>
+              <c:f>Sheet1!$B$38:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.78</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.11</c:v>
+                  <c:v>4.23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1507,7 +1536,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$54</c:f>
+              <c:f>Sheet1!$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1519,7 +1548,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$51:$D$51</c:f>
+              <c:f>Sheet1!$B$36:$D$36</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1536,19 +1565,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$54:$D$54</c:f>
+              <c:f>Sheet1!$B$39:$D$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.54</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.06</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1562,11 +1582,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="425979016"/>
-        <c:axId val="425981992"/>
+        <c:axId val="474667432"/>
+        <c:axId val="474670408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="425979016"/>
+        <c:axId val="474667432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1575,7 +1595,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425981992"/>
+        <c:crossAx val="474670408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1583,7 +1603,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425981992"/>
+        <c:axId val="474670408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1594,7 +1614,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425979016"/>
+        <c:crossAx val="474667432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1642,7 +1662,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$30</c:f>
+              <c:f>Sheet1!$A$69</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1654,7 +1674,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$29:$D$29</c:f>
+              <c:f>Sheet1!$B$68:$D$68</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1671,12 +1691,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$D$30</c:f>
+              <c:f>Sheet1!$B$69:$D$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.59</c:v>
+                  <c:v>9.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1687,11 +1713,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$31</c:f>
+              <c:f>Sheet1!$A$70</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SelectiveWeightUpdate</c:v>
+                  <c:v>AS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1699,7 +1725,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$29:$D$29</c:f>
+              <c:f>Sheet1!$B$68:$D$68</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1716,12 +1742,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$31:$D$31</c:f>
+              <c:f>Sheet1!$B$70:$D$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.23</c:v>
+                  <c:v>8.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1732,11 +1764,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$32</c:f>
+              <c:f>Sheet1!$A$71</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DiverseCritiquesWithSelectiveWtUpdate</c:v>
+                  <c:v>DIV</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1744,7 +1776,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$29:$D$29</c:f>
+              <c:f>Sheet1!$B$68:$D$68</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1761,10 +1793,19 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$32:$D$32</c:f>
+              <c:f>Sheet1!$B$71:$D$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.76</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1778,11 +1819,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="426013752"/>
-        <c:axId val="426016728"/>
+        <c:axId val="474702360"/>
+        <c:axId val="474705336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="426013752"/>
+        <c:axId val="474702360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1791,7 +1832,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="426016728"/>
+        <c:crossAx val="474705336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1799,7 +1840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="426016728"/>
+        <c:axId val="474705336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1810,7 +1851,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="426013752"/>
+        <c:crossAx val="474702360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1858,7 +1899,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$62</c:f>
+              <c:f>Sheet1!$A$76</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1870,7 +1911,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$61:$D$61</c:f>
+              <c:f>Sheet1!$B$75:$D$75</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1887,7 +1928,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$62:$D$62</c:f>
+              <c:f>Sheet1!$B$76:$D$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1909,11 +1950,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$63</c:f>
+              <c:f>Sheet1!$A$77</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AS</c:v>
+                  <c:v>MOD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1921,7 +1962,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$61:$D$61</c:f>
+              <c:f>Sheet1!$B$75:$D$75</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1938,69 +1979,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$63:$D$63</c:f>
+              <c:f>Sheet1!$B$77:$D$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.42</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.65</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.02</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$64</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DIV</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$61:$D$61</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>q1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>q3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>q5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$64:$D$64</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>7.22</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.08</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.76</c:v>
+                  <c:v>7.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2015,11 +2005,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="453884280"/>
-        <c:axId val="456141112"/>
+        <c:axId val="474732824"/>
+        <c:axId val="474735800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="453884280"/>
+        <c:axId val="474732824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2028,7 +2018,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456141112"/>
+        <c:crossAx val="474735800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2036,7 +2026,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="456141112"/>
+        <c:axId val="474735800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2047,7 +2037,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="453884280"/>
+        <c:crossAx val="474732824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2095,7 +2085,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$69</c:f>
+              <c:f>Sheet1!$A$85</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2107,7 +2097,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$68:$D$68</c:f>
+              <c:f>Sheet1!$B$84:$D$84</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2124,7 +2114,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$69:$D$69</c:f>
+              <c:f>Sheet1!$B$85:$D$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2146,11 +2136,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$70</c:f>
+              <c:f>Sheet1!$A$86</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MOD</c:v>
+                  <c:v>SIM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2158,7 +2148,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$68:$D$68</c:f>
+              <c:f>Sheet1!$B$84:$D$84</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2175,18 +2165,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$70:$D$70</c:f>
+              <c:f>Sheet1!$B$86:$D$86</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.23</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.95</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.83</c:v>
+                  <c:v>6.24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2201,11 +2191,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="454174488"/>
-        <c:axId val="435121480"/>
+        <c:axId val="474763368"/>
+        <c:axId val="474766344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="454174488"/>
+        <c:axId val="474763368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2214,7 +2204,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="435121480"/>
+        <c:crossAx val="474766344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2222,7 +2212,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="435121480"/>
+        <c:axId val="474766344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2233,7 +2223,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="454174488"/>
+        <c:crossAx val="474763368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2281,11 +2271,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$78</c:f>
+              <c:f>Sheet1!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MAUT</c:v>
+                  <c:v>MAUT-paper</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2293,7 +2283,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$77:$D$77</c:f>
+              <c:f>Sheet1!$B$2:$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2310,18 +2300,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$78:$D$78</c:f>
+              <c:f>Sheet1!$B$3:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9.05</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.91</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.24</c:v>
+                  <c:v>9.210000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2332,11 +2322,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$79</c:f>
+              <c:f>Sheet1!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SIM</c:v>
+                  <c:v>MAUT-additive</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2344,7 +2334,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$77:$D$77</c:f>
+              <c:f>Sheet1!$B$2:$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2361,18 +2351,273 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$79:$D$79</c:f>
+              <c:f>Sheet1!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.6</c:v>
+                  <c:v>8.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Diverse Critiques in Every Cycle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.38</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wMLT for nominal attributes*</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.73</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Adaptive Selection with Neutral Updates</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AdditionalPref to products satisfying critiques</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Similar Products in First Cycle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2387,11 +2632,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="434798200"/>
-        <c:axId val="462401432"/>
+        <c:axId val="474816808"/>
+        <c:axId val="474819688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="434798200"/>
+        <c:axId val="474816808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2400,7 +2645,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="462401432"/>
+        <c:crossAx val="474819688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2408,7 +2653,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="462401432"/>
+        <c:axId val="474819688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2419,14 +2664,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="434798200"/>
+        <c:crossAx val="474816808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.638931977252843"/>
+          <c:y val="0.0509470913152584"/>
+          <c:w val="0.338845800524934"/>
+          <c:h val="0.816918799237609"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2446,19 +2700,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>630619</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>166413</xdr:rowOff>
+      <xdr:colOff>490483</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>105104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2697654</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>70069</xdr:rowOff>
+      <xdr:colOff>2522482</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2476,19 +2730,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>490483</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>105104</xdr:rowOff>
+      <xdr:colOff>613103</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>116928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2522482</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>26276</xdr:rowOff>
+      <xdr:colOff>2312276</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>131380</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2506,19 +2760,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>613103</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>116928</xdr:rowOff>
+      <xdr:colOff>604344</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>122621</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2312276</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>131380</xdr:rowOff>
+      <xdr:colOff>2338551</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>183931</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2536,19 +2790,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>604344</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>122621</xdr:rowOff>
+      <xdr:colOff>376620</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>52552</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2338551</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>183931</xdr:rowOff>
+      <xdr:colOff>2539999</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>123495</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2566,19 +2820,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>376620</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>52552</xdr:rowOff>
+      <xdr:colOff>814550</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>61310</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2539999</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>123495</xdr:rowOff>
+      <xdr:colOff>1103585</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>162910</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="8" name="Chart 7"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2595,20 +2849,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>814550</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>61310</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>26276</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>8757</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1103585</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>162910</xdr:rowOff>
+      <xdr:colOff>1287517</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>40287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="9" name="Chart 8"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2626,19 +2880,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>26276</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>8757</xdr:rowOff>
+      <xdr:colOff>43791</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>105104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1287517</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>40287</xdr:rowOff>
+      <xdr:colOff>1129861</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>171669</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="10" name="Chart 9"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2656,19 +2910,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>43791</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>105104</xdr:rowOff>
+      <xdr:colOff>17518</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>21022</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1129861</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>171669</xdr:rowOff>
+      <xdr:colOff>2680139</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>75325</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvPr id="14" name="Chart 13"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3008,15 +3262,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R79"/>
+  <dimension ref="A1:R86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A79" sqref="A77:D79"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
@@ -3025,14 +3279,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="36" customHeight="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
@@ -3042,13 +3296,13 @@
       <c r="M1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
@@ -3061,9 +3315,11 @@
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" t="s">
@@ -3074,309 +3330,373 @@
       </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" s="2" customFormat="1">
       <c r="A3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="4">
-        <v>12.24</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4">
-        <v>14.54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="35" customHeight="1">
+        <v>39</v>
+      </c>
+      <c r="B3" s="12">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="C3" s="12">
+        <v>4.08</v>
+      </c>
+      <c r="D3" s="12">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3" s="11"/>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="4">
-        <v>12.8</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:18">
+        <v>37</v>
+      </c>
+      <c r="B4" s="13">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="C4" s="13">
+        <v>3.68</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1.88</v>
+      </c>
+      <c r="E4" s="18">
+        <f>ROUNDUP((B3-B4)*100/B3,1)</f>
+        <v>7.3999999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="30">
       <c r="A5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="4">
-        <v>9.1199999999999992</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="B5" s="13">
+        <v>7.83</v>
+      </c>
+      <c r="C5" s="13">
+        <v>3.12</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1.38</v>
+      </c>
+      <c r="E5" s="18">
+        <f>ROUNDUP((9.21-B5)*100/9.21,1)</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:18" ht="30">
       <c r="A6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="8">
-        <v>7.18</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8">
-        <v>8.1</v>
+        <v>41</v>
+      </c>
+      <c r="B6" s="13">
+        <v>7.13</v>
+      </c>
+      <c r="C6" s="13">
+        <v>3.45</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1.73</v>
+      </c>
+      <c r="E6" s="18">
+        <f t="shared" ref="E6:E9" si="0">ROUNDUP((9.21-B6)*100/9.21,1)</f>
+        <v>22.6</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="30">
       <c r="A7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="14">
+        <v>7.62</v>
+      </c>
+      <c r="C7" s="13">
+        <v>3.04</v>
+      </c>
+      <c r="D7" s="13">
+        <v>1.33</v>
+      </c>
+      <c r="E7" s="18">
+        <f t="shared" si="0"/>
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="30">
+      <c r="A8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="14">
+        <v>6.42</v>
+      </c>
+      <c r="C8" s="13">
+        <v>2.8</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1.37</v>
+      </c>
+      <c r="E8" s="18">
+        <f t="shared" si="0"/>
+        <v>30.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="30">
+      <c r="A9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="14">
+        <v>6.23</v>
+      </c>
+      <c r="C9" s="14">
+        <v>2.04</v>
+      </c>
+      <c r="D9" s="14">
+        <v>1.22</v>
+      </c>
+      <c r="E9" s="18">
+        <f t="shared" si="0"/>
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="14">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="C11" s="13">
+        <v>3.81</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="14">
+        <v>8.66</v>
+      </c>
+      <c r="C12" s="13">
+        <v>3.67</v>
+      </c>
+      <c r="D12" s="13">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="9"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" ht="30">
+      <c r="A15" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" ht="30">
+      <c r="A16" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="49" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="30">
+      <c r="I18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="8">
+        <v>2.15</v>
+      </c>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" ht="30">
+      <c r="I19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="8">
+        <v>3.37</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" ht="30">
+      <c r="I20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="4">
+        <v>11.34</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4">
+        <v>6.79</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4">
+        <v>8.18</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:14" s="2" customFormat="1">
+      <c r="A26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="4">
+        <v>5.52</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8">
+        <v>4.57</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:14" ht="30">
+      <c r="A28" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="8">
-        <v>8.6199999999999992</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8">
-        <v>6.94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="60">
-      <c r="A8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="8">
-        <v>6.86</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4">
-        <v>6.11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="30">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="8">
-        <v>2.15</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="30" customHeight="1">
-      <c r="A10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="8">
-        <v>3.37</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="30">
-      <c r="A11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="4">
-        <v>11.34</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="F11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="B28" s="8">
+        <v>5.64</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:14" ht="48" customHeight="1">
+      <c r="A29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="8">
+        <v>3.92</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="9" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="4">
-        <v>6.79</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:14" ht="30">
-      <c r="A18" s="9" t="s">
+      <c r="B37" s="4">
+        <v>4.59</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="4">
-        <v>8.18</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:14" s="2" customFormat="1">
-      <c r="A19" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="4">
-        <v>5.52</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" ht="30">
-      <c r="A20" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="8">
-        <v>4.57</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:14" ht="30">
-      <c r="A21" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="8">
-        <v>5.64</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:14" ht="48" customHeight="1">
-      <c r="A22" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="8">
-        <v>3.92</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="4">
-        <v>4.59</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:14" ht="30">
-      <c r="A31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="4">
+      <c r="B38" s="4">
         <v>4.2300000000000004</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:14" ht="45">
-      <c r="A32" s="6" t="s">
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" ht="30">
+      <c r="A39" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="42" spans="1:4" ht="90">
-      <c r="A42" s="7" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="49" spans="1:4" ht="60">
+      <c r="A49" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="5"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B45" s="4">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="C45" s="4">
-        <v>3.51</v>
-      </c>
-      <c r="D45" s="4">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="30">
-      <c r="A46" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="4">
-        <v>11.07</v>
-      </c>
-      <c r="C46" s="4">
-        <v>3.92</v>
-      </c>
-      <c r="D46" s="4">
-        <v>1.49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="45">
-      <c r="A47" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
+      <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>3</v>
@@ -3393,117 +3713,111 @@
         <v>18</v>
       </c>
       <c r="B52" s="4">
-        <v>3.9</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="C52" s="4">
-        <v>2.1</v>
+        <v>3.51</v>
       </c>
       <c r="D52" s="4">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="30">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="4">
-        <v>3.32</v>
+        <v>11.07</v>
       </c>
       <c r="C53" s="4">
-        <v>1.78</v>
+        <v>3.92</v>
       </c>
       <c r="D53" s="4">
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="45">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="30">
       <c r="A54" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B54" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="C54" s="4">
-        <v>1.54</v>
-      </c>
-      <c r="D54" s="4">
-        <v>1.06</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
     </row>
     <row r="57" spans="1:4">
       <c r="A57"/>
     </row>
-    <row r="60" spans="1:4" ht="30">
-      <c r="A60" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="6"/>
-      <c r="B61" s="4" t="s">
+    <row r="58" spans="1:4">
+      <c r="A58" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C58" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D58" s="3" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="C59" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="D59" s="4">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="4">
+        <v>3.32</v>
+      </c>
+      <c r="C60" s="4">
+        <v>1.78</v>
+      </c>
+      <c r="D60" s="4">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="30">
+      <c r="A61" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="C61" s="4">
+        <v>1.54</v>
+      </c>
+      <c r="D61" s="4">
+        <v>1.06</v>
+      </c>
+    </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B62" s="4">
-        <v>9.0500000000000007</v>
-      </c>
-      <c r="C62" s="4">
-        <v>3.91</v>
-      </c>
-      <c r="D62" s="4">
-        <v>2.2400000000000002</v>
-      </c>
+      <c r="A62"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B63" s="4">
-        <v>8.42</v>
-      </c>
-      <c r="C63" s="4">
-        <v>3.65</v>
-      </c>
-      <c r="D63" s="4">
-        <v>2.02</v>
-      </c>
+      <c r="A63"/>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B64" s="4">
-        <v>7.22</v>
-      </c>
-      <c r="C64" s="4">
-        <v>3.08</v>
-      </c>
-      <c r="D64" s="4">
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="45">
+      <c r="A64"/>
+    </row>
+    <row r="67" spans="1:4" ht="30">
       <c r="A67" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -3534,60 +3848,119 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B70" s="4">
+        <v>8.42</v>
+      </c>
+      <c r="C70" s="4">
+        <v>3.65</v>
+      </c>
+      <c r="D70" s="4">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="4">
+        <v>7.22</v>
+      </c>
+      <c r="C71" s="4">
+        <v>3.08</v>
+      </c>
+      <c r="D71" s="4">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="30">
+      <c r="A74" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="6"/>
+      <c r="B75" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76" s="4">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="C76" s="4">
+        <v>3.91</v>
+      </c>
+      <c r="D76" s="4">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B77" s="4">
         <v>7.23</v>
       </c>
-      <c r="C70" s="4">
+      <c r="C77" s="4">
         <v>2.95</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D77" s="4">
         <v>1.83</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="30">
-      <c r="A76" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="6"/>
-      <c r="B77" s="4" t="s">
+    <row r="83" spans="1:4">
+      <c r="A83" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="6"/>
+      <c r="B84" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C84" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D84" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="6" t="s">
+    <row r="85" spans="1:4">
+      <c r="A85" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B78" s="4">
+      <c r="B85" s="4">
         <v>9.0500000000000007</v>
       </c>
-      <c r="C78" s="4">
+      <c r="C85" s="4">
         <v>3.91</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D85" s="4">
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B79" s="4">
+    <row r="86" spans="1:4">
+      <c r="A86" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B86" s="4">
         <v>6.24</v>
       </c>
-      <c r="C79" s="4">
+      <c r="C86" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D86" s="4">
         <v>1.6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Market equilibrium modification added. Shows 4% improvement on both camera and PC data sets
</commit_message>
<xml_diff>
--- a/src/Results.xlsx
+++ b/src/Results.xlsx
@@ -627,7 +627,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$24</c:f>
+              <c:f>Sheet1!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -639,7 +639,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$23:$D$23</c:f>
+              <c:f>Sheet1!$B$22:$D$22</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -656,7 +656,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$24:$D$24</c:f>
+              <c:f>Sheet1!$B$23:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -672,7 +672,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$25</c:f>
+              <c:f>Sheet1!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -684,7 +684,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$23:$D$23</c:f>
+              <c:f>Sheet1!$B$22:$D$22</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -701,7 +701,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$25:$D$25</c:f>
+              <c:f>Sheet1!$B$24:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -717,7 +717,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$26</c:f>
+              <c:f>Sheet1!$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -729,7 +729,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$23:$D$23</c:f>
+              <c:f>Sheet1!$B$22:$D$22</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -746,7 +746,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$26:$D$26</c:f>
+              <c:f>Sheet1!$B$25:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -762,7 +762,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$27</c:f>
+              <c:f>Sheet1!$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -774,7 +774,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$23:$D$23</c:f>
+              <c:f>Sheet1!$B$22:$D$22</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -791,7 +791,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$27:$D$27</c:f>
+              <c:f>Sheet1!$B$26:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -807,7 +807,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$28</c:f>
+              <c:f>Sheet1!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -819,7 +819,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$23:$D$23</c:f>
+              <c:f>Sheet1!$B$22:$D$22</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -836,7 +836,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$28:$D$28</c:f>
+              <c:f>Sheet1!$B$27:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -852,7 +852,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$29</c:f>
+              <c:f>Sheet1!$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -864,7 +864,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$23:$D$23</c:f>
+              <c:f>Sheet1!$B$22:$D$22</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -881,7 +881,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$29:$D$29</c:f>
+              <c:f>Sheet1!$B$28:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -981,7 +981,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$52</c:f>
+              <c:f>Sheet1!$A$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -993,7 +993,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$51:$D$51</c:f>
+              <c:f>Sheet1!$B$50:$D$50</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1010,7 +1010,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$52:$D$52</c:f>
+              <c:f>Sheet1!$B$51:$D$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1032,7 +1032,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$53</c:f>
+              <c:f>Sheet1!$A$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1044,7 +1044,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$51:$D$51</c:f>
+              <c:f>Sheet1!$B$50:$D$50</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1061,7 +1061,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$53:$D$53</c:f>
+              <c:f>Sheet1!$B$52:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1083,7 +1083,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$54</c:f>
+              <c:f>Sheet1!$A$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1095,7 +1095,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$51:$D$51</c:f>
+              <c:f>Sheet1!$B$50:$D$50</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1112,7 +1112,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$54:$D$54</c:f>
+              <c:f>Sheet1!$B$53:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1209,7 +1209,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$59</c:f>
+              <c:f>Sheet1!$A$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1221,7 +1221,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$58:$D$58</c:f>
+              <c:f>Sheet1!$B$57:$D$57</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1238,7 +1238,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$59:$D$59</c:f>
+              <c:f>Sheet1!$B$58:$D$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1260,7 +1260,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$60</c:f>
+              <c:f>Sheet1!$A$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1272,7 +1272,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$58:$D$58</c:f>
+              <c:f>Sheet1!$B$57:$D$57</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1289,7 +1289,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$60:$D$60</c:f>
+              <c:f>Sheet1!$B$59:$D$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1311,7 +1311,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$61</c:f>
+              <c:f>Sheet1!$A$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1323,7 +1323,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$58:$D$58</c:f>
+              <c:f>Sheet1!$B$57:$D$57</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1340,7 +1340,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$61:$D$61</c:f>
+              <c:f>Sheet1!$B$60:$D$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1446,7 +1446,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$37</c:f>
+              <c:f>Sheet1!$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1458,7 +1458,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$36:$D$36</c:f>
+              <c:f>Sheet1!$B$35:$D$35</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1475,7 +1475,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$37:$D$37</c:f>
+              <c:f>Sheet1!$B$36:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1491,7 +1491,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$38</c:f>
+              <c:f>Sheet1!$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1503,7 +1503,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$36:$D$36</c:f>
+              <c:f>Sheet1!$B$35:$D$35</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1520,7 +1520,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$38:$D$38</c:f>
+              <c:f>Sheet1!$B$37:$D$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1536,7 +1536,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$39</c:f>
+              <c:f>Sheet1!$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1548,7 +1548,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$36:$D$36</c:f>
+              <c:f>Sheet1!$B$35:$D$35</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1565,7 +1565,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$39:$D$39</c:f>
+              <c:f>Sheet1!$B$38:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1662,7 +1662,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$69</c:f>
+              <c:f>Sheet1!$A$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1674,7 +1674,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$68:$D$68</c:f>
+              <c:f>Sheet1!$B$67:$D$67</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1691,7 +1691,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$69:$D$69</c:f>
+              <c:f>Sheet1!$B$68:$D$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1713,7 +1713,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$70</c:f>
+              <c:f>Sheet1!$A$69</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1725,7 +1725,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$68:$D$68</c:f>
+              <c:f>Sheet1!$B$67:$D$67</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1742,7 +1742,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$70:$D$70</c:f>
+              <c:f>Sheet1!$B$69:$D$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1764,7 +1764,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$71</c:f>
+              <c:f>Sheet1!$A$70</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1776,7 +1776,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$68:$D$68</c:f>
+              <c:f>Sheet1!$B$67:$D$67</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1793,7 +1793,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$71:$D$71</c:f>
+              <c:f>Sheet1!$B$70:$D$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1899,7 +1899,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$76</c:f>
+              <c:f>Sheet1!$A$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1911,7 +1911,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$75:$D$75</c:f>
+              <c:f>Sheet1!$B$74:$D$74</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1928,7 +1928,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$76:$D$76</c:f>
+              <c:f>Sheet1!$B$75:$D$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1950,7 +1950,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$77</c:f>
+              <c:f>Sheet1!$A$76</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1962,7 +1962,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$75:$D$75</c:f>
+              <c:f>Sheet1!$B$74:$D$74</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1979,7 +1979,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$77:$D$77</c:f>
+              <c:f>Sheet1!$B$76:$D$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2085,7 +2085,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$85</c:f>
+              <c:f>Sheet1!$A$84</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2097,7 +2097,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$84:$D$84</c:f>
+              <c:f>Sheet1!$B$83:$D$83</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2114,7 +2114,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$85:$D$85</c:f>
+              <c:f>Sheet1!$B$84:$D$84</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2136,7 +2136,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$86</c:f>
+              <c:f>Sheet1!$A$85</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2148,7 +2148,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$84:$D$84</c:f>
+              <c:f>Sheet1!$B$83:$D$83</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2165,7 +2165,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$86:$D$86</c:f>
+              <c:f>Sheet1!$B$85:$D$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2356,7 +2356,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.53</c:v>
+                  <c:v>8.720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.68</c:v>
@@ -2701,13 +2701,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>490483</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>105104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2522482</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>26276</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2731,13 +2731,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>613103</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>116928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2312276</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>131380</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2761,13 +2761,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>604344</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>122621</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2338551</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>183931</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2791,13 +2791,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>376620</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>52552</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2539999</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>123495</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2821,13 +2821,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>814550</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>61310</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1103585</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>162910</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2851,13 +2851,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>26276</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>8757</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1287517</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>40287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2881,13 +2881,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>43791</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>105104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1129861</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>171669</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3262,10 +3262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R86"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3355,7 +3355,7 @@
         <v>37</v>
       </c>
       <c r="B4" s="13">
-        <v>8.5299999999999994</v>
+        <v>8.7200000000000006</v>
       </c>
       <c r="C4" s="13">
         <v>3.68</v>
@@ -3365,7 +3365,7 @@
       </c>
       <c r="E4" s="18">
         <f>ROUNDUP((B3-B4)*100/B3,1)</f>
-        <v>7.3999999999999995</v>
+        <v>5.3999999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="30">
@@ -3493,315 +3493,324 @@
       <c r="A13" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="9"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="B13" s="4">
+        <v>8.51</v>
+      </c>
+      <c r="C13" s="4">
+        <v>3.51</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="30">
+      <c r="A14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="4">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="C14" s="4">
+        <v>4.42</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2.41</v>
+      </c>
     </row>
     <row r="15" spans="1:18" ht="30">
-      <c r="A15" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:18" ht="30">
-      <c r="A16" s="15" t="s">
+      <c r="A15" s="15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="49" customHeight="1">
-      <c r="A17" s="2" t="s">
+    <row r="16" spans="1:18" ht="49" customHeight="1">
+      <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>50</v>
       </c>
     </row>
+    <row r="17" spans="1:14" ht="30">
+      <c r="I17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="8">
+        <v>2.15</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
     <row r="18" spans="1:14" ht="30">
-      <c r="I18" s="6" t="s">
-        <v>24</v>
+      <c r="I18" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="J18" s="8">
-        <v>2.15</v>
+        <v>3.37</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:14" ht="30">
-      <c r="I19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="8">
-        <v>3.37</v>
+      <c r="I19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="4">
+        <v>11.34</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:14" ht="30">
-      <c r="I20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" s="4">
-        <v>11.34</v>
-      </c>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
+    <row r="22" spans="1:14">
+      <c r="A22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="4">
+        <v>6.79</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" s="4">
-        <v>6.79</v>
+        <v>8.18</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" s="2" customFormat="1">
       <c r="A25" s="9" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B25" s="4">
-        <v>8.18</v>
+        <v>5.52</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:14" s="2" customFormat="1">
+    <row r="26" spans="1:14">
       <c r="A26" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="4">
-        <v>5.52</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:14">
+        <v>26</v>
+      </c>
+      <c r="B26" s="8">
+        <v>4.57</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:14" ht="30">
       <c r="A27" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B27" s="8">
-        <v>4.57</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:14" ht="30">
+        <v>5.64</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" ht="48" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B28" s="8">
-        <v>5.64</v>
+        <v>3.92</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:14" ht="48" customHeight="1">
-      <c r="A29" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="8">
-        <v>3.92</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2" t="s">
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="L28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="M28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N29" s="2" t="s">
+      <c r="N28" s="2" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A36" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="4">
+        <v>4.59</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B37" s="4">
-        <v>4.59</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" ht="30">
       <c r="A38" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="4">
-        <v>4.2300000000000004</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:4" ht="30">
-      <c r="A39" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="49" spans="1:4" ht="60">
-      <c r="A49" s="7" t="s">
+    <row r="48" spans="1:4" ht="60">
+      <c r="A48" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="5"/>
       <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="5"/>
-      <c r="B50" s="2"/>
+      <c r="A50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>5</v>
+      <c r="A51" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="C51" s="4">
+        <v>3.51</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1.35</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="4">
+        <v>11.07</v>
+      </c>
+      <c r="C52" s="4">
+        <v>3.92</v>
+      </c>
+      <c r="D52" s="4">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30">
+      <c r="A53" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B52" s="4">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="C52" s="4">
-        <v>3.51</v>
-      </c>
-      <c r="D52" s="4">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B53" s="4">
-        <v>11.07</v>
-      </c>
-      <c r="C53" s="4">
-        <v>3.92</v>
-      </c>
-      <c r="D53" s="4">
-        <v>1.49</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="30">
-      <c r="A54" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>5</v>
+      <c r="B58" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="C58" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="D58" s="4">
+        <v>1.23</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B59" s="4">
-        <v>3.9</v>
+        <v>3.32</v>
       </c>
       <c r="C59" s="4">
-        <v>2.1</v>
+        <v>1.78</v>
       </c>
       <c r="D59" s="4">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="30">
       <c r="A60" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B60" s="4">
-        <v>3.32</v>
+        <v>3.2</v>
       </c>
       <c r="C60" s="4">
-        <v>1.78</v>
+        <v>1.54</v>
       </c>
       <c r="D60" s="4">
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="30">
-      <c r="A61" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B61" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="C61" s="4">
-        <v>1.54</v>
-      </c>
-      <c r="D61" s="4">
         <v>1.06</v>
       </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62"/>
@@ -3809,158 +3818,155 @@
     <row r="63" spans="1:4">
       <c r="A63"/>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64"/>
-    </row>
-    <row r="67" spans="1:4" ht="30">
-      <c r="A67" s="2" t="s">
+    <row r="66" spans="1:4" ht="30">
+      <c r="A66" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>31</v>
       </c>
     </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="6"/>
+      <c r="B67" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="6"/>
-      <c r="B68" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>5</v>
+      <c r="A68" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" s="4">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="C68" s="4">
+        <v>3.91</v>
+      </c>
+      <c r="D68" s="4">
+        <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="6" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B69" s="4">
-        <v>9.0500000000000007</v>
+        <v>8.42</v>
       </c>
       <c r="C69" s="4">
-        <v>3.91</v>
+        <v>3.65</v>
       </c>
       <c r="D69" s="4">
-        <v>2.2400000000000002</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B70" s="4">
-        <v>8.42</v>
+        <v>7.22</v>
       </c>
       <c r="C70" s="4">
-        <v>3.65</v>
+        <v>3.08</v>
       </c>
       <c r="D70" s="4">
-        <v>2.02</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" s="4">
-        <v>7.22</v>
-      </c>
-      <c r="C71" s="4">
-        <v>3.08</v>
-      </c>
-      <c r="D71" s="4">
         <v>1.76</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="30">
-      <c r="A74" s="2" t="s">
+    <row r="73" spans="1:4" ht="30">
+      <c r="A73" s="2" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="6"/>
+      <c r="B74" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="6"/>
-      <c r="B75" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>5</v>
+      <c r="A75" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75" s="4">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="C75" s="4">
+        <v>3.91</v>
+      </c>
+      <c r="D75" s="4">
+        <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76" s="4">
+        <v>7.23</v>
+      </c>
+      <c r="C76" s="4">
+        <v>2.95</v>
+      </c>
+      <c r="D76" s="4">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="6"/>
+      <c r="B83" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B84" s="4">
         <v>9.0500000000000007</v>
       </c>
-      <c r="C76" s="4">
+      <c r="C84" s="4">
         <v>3.91</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D84" s="4">
         <v>2.2400000000000002</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B77" s="4">
-        <v>7.23</v>
-      </c>
-      <c r="C77" s="4">
-        <v>2.95</v>
-      </c>
-      <c r="D77" s="4">
-        <v>1.83</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="6"/>
-      <c r="B84" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="6" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B85" s="4">
-        <v>9.0500000000000007</v>
+        <v>6.24</v>
       </c>
       <c r="C85" s="4">
-        <v>3.91</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D85" s="4">
-        <v>2.2400000000000002</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B86" s="4">
-        <v>6.24</v>
-      </c>
-      <c r="C86" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D86" s="4">
         <v>1.6</v>
       </c>
     </row>

</xml_diff>